<commit_message>
Converted from static to flask webapp
</commit_message>
<xml_diff>
--- a/static/data/data.xlsx
+++ b/static/data/data.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrey/Documents/Charu Arora/charuaroraofficial.github.io/static/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82552D6-609A-994F-BA19-2A6532B6A11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="index_page" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="collection_list" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="lehengas" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Bridal gowns" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Saree and Drapes" sheetId="5" r:id="rId8"/>
+    <sheet name="index_page" sheetId="1" r:id="rId1"/>
+    <sheet name="collection_list" sheetId="2" r:id="rId2"/>
+    <sheet name="lehengas" sheetId="3" r:id="rId3"/>
+    <sheet name="Bridal gowns" sheetId="4" r:id="rId4"/>
+    <sheet name="Saree and Drapes" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Content</t>
   </si>
@@ -47,9 +56,6 @@
     <t>somethingfor3</t>
   </si>
   <si>
-    <t>Lehanga</t>
-  </si>
-  <si>
     <t>Bridal gowns</t>
   </si>
   <si>
@@ -97,32 +103,63 @@
   <si>
     <t>Discover elegance in our pink lehenga crafted from premium net fabric. Adorned with meticulous detailing including sequins, cut dana, crystals and miroor work, this ensemble excudes sophistication. Paired with a matching net dupatta, its a celebration of timeless craftsmanship and contemporary style. Elevate your ethnic wardrobe with this opulent creation.</t>
   </si>
+  <si>
+    <t>lehengas</t>
+  </si>
+  <si>
+    <t>collection_type</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -130,7 +167,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -140,57 +177,47 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -380,25 +407,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.63"/>
-    <col customWidth="1" min="2" max="2" width="15.0"/>
-    <col customWidth="1" min="3" max="3" width="7.25"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,12 +439,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -422,10 +452,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>30000.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -433,10 +463,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>20000.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -444,144 +474,159 @@
         <v>9</v>
       </c>
       <c r="C5" s="2">
-        <v>10000.0</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4">
+        <v>90000</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4">
+        <v>90000</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4">
-        <v>90000.0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="4">
-        <v>90000.0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>